<commit_message>
cell macro will return integers if the value is a long sized and does not have a fraction range macro was developed, tests were created and documented
</commit_message>
<xml_diff>
--- a/jamal-xls/README.xlsx
+++ b/jamal-xls/README.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verhasp/github/jamal/jamal-xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FED372-2B97-1C47-AD47-F763910710B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D700540-8C17-E34C-BB78-B2EAC8E6F655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16240" yWindow="7380" windowWidth="28040" windowHeight="17440" xr2:uid="{5FA2AFD4-335A-3246-B938-841A5EE25EAD}"/>
+    <workbookView xWindow="16240" yWindow="7380" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{5FA2AFD4-335A-3246-B938-841A5EE25EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="MULTI" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="CellName">README!$A$1</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>A</t>
   </si>
@@ -59,13 +60,119 @@
   </si>
   <si>
     <t>third will get to the second column</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Year of publishing</t>
+  </si>
+  <si>
+    <t>Pride and Prejudice</t>
+  </si>
+  <si>
+    <t>Jane Austen</t>
+  </si>
+  <si>
+    <t>T. Egerton</t>
+  </si>
+  <si>
+    <t>Moby-Dick</t>
+  </si>
+  <si>
+    <t>Herman Melville</t>
+  </si>
+  <si>
+    <t>Harper &amp; Brothers</t>
+  </si>
+  <si>
+    <t>Adventures of Huckleberry Finn</t>
+  </si>
+  <si>
+    <t>Mark Twain</t>
+  </si>
+  <si>
+    <t>Charles L. Webster and Company</t>
+  </si>
+  <si>
+    <t>The Picture of Dorian Gray</t>
+  </si>
+  <si>
+    <t>Oscar Wilde</t>
+  </si>
+  <si>
+    <t>Lippincott's Monthly Magazine</t>
+  </si>
+  <si>
+    <t>Dracula</t>
+  </si>
+  <si>
+    <t>Bram Stoker</t>
+  </si>
+  <si>
+    <t>Archibald Constable and Company</t>
+  </si>
+  <si>
+    <t>The War of the Worlds</t>
+  </si>
+  <si>
+    <t>H.G. Wells</t>
+  </si>
+  <si>
+    <t>William Heinemann</t>
+  </si>
+  <si>
+    <t>Heart of Darkness</t>
+  </si>
+  <si>
+    <t>Joseph Conrad</t>
+  </si>
+  <si>
+    <t>Blackwood's Magazine</t>
+  </si>
+  <si>
+    <t>The Wonderful Wizard of Oz</t>
+  </si>
+  <si>
+    <t>L. Frank Baum</t>
+  </si>
+  <si>
+    <t>George M. Hill Company</t>
+  </si>
+  <si>
+    <t>The Call of the Wild</t>
+  </si>
+  <si>
+    <t>Jack London</t>
+  </si>
+  <si>
+    <t>Macmillan</t>
+  </si>
+  <si>
+    <t>A Room with a View</t>
+  </si>
+  <si>
+    <t>E.M. Forster</t>
+  </si>
+  <si>
+    <t>Edward Arnold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +194,29 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -102,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,19 +240,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AEB8E2-D051-7446-9F43-E52F39AB36A8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -629,4 +781,183 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FCC2B6-97F7-8041-8720-1512A552C379}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>